<commit_message>
July 28 @11:02am - updating csv file
</commit_message>
<xml_diff>
--- a/census_viz/pet_ownership.xlsx
+++ b/census_viz/pet_ownership.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minaakbari/CS6017/census_viz/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minaakbari/HW_7_Pet_State/census_viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9990374-D120-C54A-9227-4460A35F7FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4173DE82-9D48-F943-912F-EC7184DBB100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16680" xr2:uid="{4D13B6C1-5EF3-EF4C-993E-8F72D848B145}"/>
   </bookViews>
@@ -50,148 +50,148 @@
     <t>CatOwnershipRate</t>
   </si>
   <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>Delaware</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Idaho</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>Iowa</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>Maine</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>Montana</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>New Hampshire</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
-    <t>North Dakota</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>Rhode Island</t>
-  </si>
-  <si>
-    <t>South Carolina</t>
-  </si>
-  <si>
-    <t>South Dakota</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>West Virginia</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
+    <t>alabama</t>
+  </si>
+  <si>
+    <t>arizona</t>
+  </si>
+  <si>
+    <t>arkansas</t>
+  </si>
+  <si>
+    <t>california</t>
+  </si>
+  <si>
+    <t>colorado</t>
+  </si>
+  <si>
+    <t>connecticut</t>
+  </si>
+  <si>
+    <t>delaware</t>
+  </si>
+  <si>
+    <t>florida</t>
+  </si>
+  <si>
+    <t>georgia</t>
+  </si>
+  <si>
+    <t>idaho</t>
+  </si>
+  <si>
+    <t>illinois</t>
+  </si>
+  <si>
+    <t>indiana</t>
+  </si>
+  <si>
+    <t>wyoming</t>
+  </si>
+  <si>
+    <t>wisconsin</t>
+  </si>
+  <si>
+    <t>west Virginia</t>
+  </si>
+  <si>
+    <t>washington</t>
+  </si>
+  <si>
+    <t>virginia</t>
+  </si>
+  <si>
+    <t>vermont</t>
+  </si>
+  <si>
+    <t>utah</t>
+  </si>
+  <si>
+    <t>texas</t>
+  </si>
+  <si>
+    <t>tennessee</t>
+  </si>
+  <si>
+    <t>south dakota</t>
+  </si>
+  <si>
+    <t>south carolina</t>
+  </si>
+  <si>
+    <t>rhode island</t>
+  </si>
+  <si>
+    <t>pennsylvania</t>
+  </si>
+  <si>
+    <t>oregon</t>
+  </si>
+  <si>
+    <t>oklahoma</t>
+  </si>
+  <si>
+    <t>ohio</t>
+  </si>
+  <si>
+    <t>north dakota</t>
+  </si>
+  <si>
+    <t>north carolina</t>
+  </si>
+  <si>
+    <t>new york</t>
+  </si>
+  <si>
+    <t>new mexico</t>
+  </si>
+  <si>
+    <t>new jersey</t>
+  </si>
+  <si>
+    <t>new hampshire</t>
+  </si>
+  <si>
+    <t>nevada</t>
+  </si>
+  <si>
+    <t>nebraska</t>
+  </si>
+  <si>
+    <t>montana</t>
+  </si>
+  <si>
+    <t>missouri</t>
+  </si>
+  <si>
+    <t>mississippi</t>
+  </si>
+  <si>
+    <t>minnesota</t>
+  </si>
+  <si>
+    <t>michigan</t>
+  </si>
+  <si>
+    <t>massachusetts</t>
+  </si>
+  <si>
+    <t>maryland</t>
+  </si>
+  <si>
+    <t>maine</t>
+  </si>
+  <si>
+    <t>louisiana</t>
+  </si>
+  <si>
+    <t>kentucky</t>
+  </si>
+  <si>
+    <t>kansas</t>
+  </si>
+  <si>
+    <t>iowa</t>
   </si>
 </sst>
 </file>
@@ -580,11 +580,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566F4929-894A-6A4B-8B22-F7967E9F6CA0}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="4" width="22.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -770,7 +775,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2">
         <v>59</v>
@@ -784,7 +789,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B15" s="2">
         <v>62.8</v>
@@ -798,7 +803,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2">
         <v>64.099999999999994</v>
@@ -812,7 +817,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2">
         <v>54</v>
@@ -826,7 +831,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2">
         <v>63.5</v>
@@ -840,7 +845,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B19" s="2">
         <v>48.6</v>
@@ -854,7 +859,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B20" s="2">
         <v>49</v>
@@ -868,7 +873,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2">
         <v>62.4</v>
@@ -882,7 +887,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2">
         <v>54</v>
@@ -896,7 +901,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2">
         <v>65.5</v>
@@ -910,7 +915,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2">
         <v>63.5</v>
@@ -924,7 +929,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B25" s="2">
         <v>62</v>
@@ -938,7 +943,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B26" s="2">
         <v>51.3</v>
@@ -952,7 +957,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B27" s="2">
         <v>53</v>
@@ -966,7 +971,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B28" s="2">
         <v>52</v>
@@ -980,7 +985,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B29" s="2">
         <v>47.4</v>
@@ -994,7 +999,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B30" s="2">
         <v>60</v>
@@ -1008,7 +1013,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="2">
         <v>50</v>
@@ -1022,7 +1027,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="2">
         <v>59</v>
@@ -1036,7 +1041,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2">
         <v>63.7</v>
@@ -1050,7 +1055,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B34" s="2">
         <v>62.4</v>
@@ -1064,7 +1069,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B35" s="2">
         <v>65</v>
@@ -1078,7 +1083,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B36" s="2">
         <v>59.2</v>
@@ -1092,7 +1097,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B37" s="2">
         <v>60.6</v>
@@ -1106,7 +1111,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B38" s="2">
         <v>45.4</v>
@@ -1120,7 +1125,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B39" s="2">
         <v>62</v>
@@ -1134,7 +1139,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B40" s="2">
         <v>46</v>
@@ -1148,7 +1153,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B41" s="2">
         <v>61.7</v>
@@ -1162,7 +1167,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B42" s="2">
         <v>58.2</v>
@@ -1176,7 +1181,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B43" s="2">
         <v>58.5</v>
@@ -1190,7 +1195,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B44" s="2">
         <v>70</v>
@@ -1204,7 +1209,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="B45" s="2">
         <v>55.5</v>
@@ -1218,7 +1223,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="B46" s="2">
         <v>63</v>
@@ -1232,7 +1237,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B47" s="2">
         <v>71</v>
@@ -1246,7 +1251,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B48" s="2">
         <v>59</v>
@@ -1260,7 +1265,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B49" s="2">
         <v>71.8</v>

</xml_diff>

<commit_message>
July 28 @7:16pm - Highlight, pop up, green_color
</commit_message>
<xml_diff>
--- a/census_viz/pet_ownership.xlsx
+++ b/census_viz/pet_ownership.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minaakbari/HW_7_Pet_State/census_viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4173DE82-9D48-F943-912F-EC7184DBB100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B2F0E1-D4DF-A740-B992-7C083A50AB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16680" xr2:uid="{4D13B6C1-5EF3-EF4C-993E-8F72D848B145}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>State</t>
   </si>
@@ -192,13 +192,19 @@
   </si>
   <si>
     <t>iowa</t>
+  </si>
+  <si>
+    <t>hawaii</t>
+  </si>
+  <si>
+    <t>alaska</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -218,6 +224,13 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -240,10 +253,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566F4929-894A-6A4B-8B22-F7967E9F6CA0}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1277,6 +1291,16 @@
         <v>30</v>
       </c>
     </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>